<commit_message>
Update module Inventario: update documents remision
</commit_message>
<xml_diff>
--- a/static/documentos/despacho_1.xlsx
+++ b/static/documentos/despacho_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PycharmProjects\uni2data\static\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm\uni2data\static\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE00E426-D93D-4749-87B6-30B8A8479B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD43CE4-4E5C-4AA1-BD53-A18F4CAE25B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DD838A3A-8495-4C03-BF2E-9AF1D86AFF1C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>REMISIÓN</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>AIMER CARDENAS</t>
+  </si>
+  <si>
+    <t>MARCA</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -484,30 +487,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -651,6 +630,37 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -660,313 +670,310 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1351,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C2C35D-678A-4093-B4D8-F4B5FA78B74D}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="A1:J37"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,505 +1371,543 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="81"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="30" t="s">
+      <c r="D6" s="52"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="36"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="91"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="37" t="s">
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="44"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="51"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="37" t="s">
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46" t="s">
+      <c r="E8" s="46"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="47"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="50"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="61"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="28" t="s">
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="57" t="s">
+      <c r="I11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="98" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="63"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="100"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="67"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="102"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="67"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="102"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="67"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="102"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="67"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="102"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="67"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="102"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="67"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="102"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="67"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="102"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="67"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="102"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="67"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="102"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="67"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="96"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="102"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="67"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="101"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="102"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="67"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="101"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="102"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="67"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="101"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="102"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="64"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="67"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="102"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="64"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="67"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="101"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="102"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="67"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="102"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="64"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="67"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="102"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="72"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="67"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="105"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="102"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="77"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="78" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="79"/>
-      <c r="J31" s="80"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="81"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="82" t="s">
+      <c r="A32" s="37"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="83"/>
-      <c r="J32" s="84"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="14"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="86" t="s">
+      <c r="A33" s="32"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="87"/>
-      <c r="J33" s="80"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="88" t="s">
+      <c r="A34" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="89"/>
-      <c r="C34" s="90" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="91"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="90" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G34" s="91"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="77" t="s">
+      <c r="G34" s="16"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="J34" s="93"/>
+      <c r="J34" s="31"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="94"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="96" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="97"/>
-      <c r="E35" s="98"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="98"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="99"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="94"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="96"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="100" t="s">
+      <c r="A36" s="26"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J36" s="101"/>
+      <c r="J36" s="35"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="102"/>
-      <c r="B37" s="103"/>
-      <c r="C37" s="104"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="106"/>
-      <c r="F37" s="104"/>
-      <c r="G37" s="105"/>
-      <c r="H37" s="106"/>
-      <c r="I37" s="104"/>
-      <c r="J37" s="106"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="A1:B5"/>
+    <mergeCell ref="C1:F5"/>
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="G3:J5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:J10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="A31:G33"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E37"/>
     <mergeCell ref="A34:B34"/>
@@ -1873,42 +1918,6 @@
     <mergeCell ref="I37:J37"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="F35:H37"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="A31:G33"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A9:J10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="C1:F5"/>
-    <mergeCell ref="G1:J2"/>
-    <mergeCell ref="G3:J5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="portrait" r:id="rId1"/>

</xml_diff>